<commit_message>
fourth test added and page.locators added
</commit_message>
<xml_diff>
--- a/Redmine_test-cases.xlsx
+++ b/Redmine_test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\redmine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD925C0-2AF3-458A-8816-FA9AE344E48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41509B3B-5050-4817-9A66-EACF72C5D19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{4DB275C8-9FF3-4DE1-91B9-7F6B779C0F23}"/>
   </bookViews>
@@ -78,9 +78,6 @@
 2. Search input: "haskell"</t>
   </si>
   <si>
-    <t>Adding an "Author" column for issues on the "Options" part from the "Issues" tab and applying the changes</t>
-  </si>
-  <si>
     <t>1. Click on the "Issues" tab
 2. Click on the "Options" scope
 3. Click on the "Author" opiton
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Checking the correct order of forums and the presence of links from "Forums" tab</t>
+  </si>
+  <si>
+    <t>Adding an "Author" column for issues from the "Issues" tab and applying the changes</t>
   </si>
 </sst>
 </file>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1090D055-DAD5-4E71-AEED-147592CD9B0B}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,13 +597,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="94.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -611,16 +611,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -637,7 +637,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -645,16 +645,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="64" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -662,16 +662,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">

</xml_diff>